<commit_message>
imported probes for LaJara_2022
</commit_message>
<xml_diff>
--- a/Topography/LaJara_TopoSurvey/LongProfile_Analysis.xlsx
+++ b/Topography/LaJara_TopoSurvey/LongProfile_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615DFD94-DD3C-4A01-9A18-579A8E70D55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB0F257-9141-44C4-9FB2-D9539ACB1EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" firstSheet="1" activeTab="6" xr2:uid="{03481A16-4B90-474B-945E-1D75A00D1B70}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{03481A16-4B90-474B-945E-1D75A00D1B70}"/>
   </bookViews>
   <sheets>
     <sheet name="TP1 (3&amp;25)" sheetId="4" r:id="rId1"/>
@@ -608,9 +608,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -624,6 +621,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3199,6 +3199,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-96E7-4774-956D-5A8411B275E3}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11167,84 +11170,84 @@
       <c r="C13" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
+      <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16" s="19">
         <v>2722.69</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="19">
         <v>13</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="19">
         <v>2722.4960000000001</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
+      <c r="A18" s="19">
         <v>13</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="19">
         <f>B17-1</f>
         <v>2721.4960000000001</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="A21" s="20">
         <v>13</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="19">
         <v>2722.652</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="20" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="21">
+      <c r="A22" s="20">
         <v>13</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" s="19">
         <v>2722.5129999999999</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="20" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
+      <c r="A23" s="20">
         <v>13</v>
       </c>
-      <c r="B23" s="20">
+      <c r="B23" s="19">
         <f>B22-1</f>
         <v>2721.5129999999999</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="20" t="s">
         <v>91</v>
       </c>
     </row>
@@ -11797,36 +11800,36 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
+      <c r="A18" s="19">
         <v>23</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="19">
         <v>2723.3890000000001</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
+      <c r="A19" s="19">
         <v>23</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="19">
         <v>2723.1850000000004</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
+      <c r="A20" s="19">
         <v>23</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="19">
         <f>B19-1</f>
         <v>2722.1850000000004</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>91</v>
       </c>
     </row>
@@ -11936,13 +11939,13 @@
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="21">
         <v>41</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="21">
         <v>2724.7139999999995</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>125</v>
       </c>
     </row>
@@ -11960,36 +11963,36 @@
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
+      <c r="A12" s="19">
         <v>41</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="19">
         <v>2724.88</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="20">
+      <c r="A13" s="19">
         <v>41</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="19">
         <v>2724.6550000000002</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+      <c r="A14" s="19">
         <v>41</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="19">
         <f>B13-1</f>
         <v>2723.6550000000002</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12174,36 +12177,36 @@
       <c r="C15" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="19">
         <v>10.15</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="19">
         <v>2733.665</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
+      <c r="A18" s="19">
         <v>10.15</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="19">
         <v>2733.5459999999998</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
+      <c r="A19" s="19">
         <v>10.15</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="19">
         <f>B18-1</f>
         <v>2732.5459999999998</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12363,36 +12366,36 @@
       <c r="C15" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="19">
         <v>14.600000000000001</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="22">
         <v>2733.998</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
+      <c r="A18" s="19">
         <v>14.600000000000001</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="19">
         <v>2733.8110000000001</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
+      <c r="A19" s="19">
         <v>14.600000000000001</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="19">
         <f>B18-1</f>
         <v>2732.8110000000001</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12575,36 +12578,36 @@
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="19">
         <v>31.4</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="22">
         <v>2735.6690000000003</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
+      <c r="A18" s="19">
         <v>31.4</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="19">
         <v>2735.3720000000003</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
+      <c r="A19" s="19">
         <v>31.4</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="19">
         <f>B18-1</f>
         <v>2734.3720000000003</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>91</v>
       </c>
     </row>
@@ -12772,84 +12775,84 @@
       <c r="C16" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="24">
+      <c r="A19" s="23">
         <v>56.599999999999994</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="22">
         <v>2738.5079999999998</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="19" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="24">
+      <c r="A20" s="23">
         <v>56.599999999999994</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="19">
         <v>2738.3150000000001</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="24">
+      <c r="A21" s="23">
         <v>56.599999999999994</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="19">
         <f>B20-1</f>
         <v>2737.3150000000001</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="19" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="24">
+      <c r="A25" s="23">
         <v>56.599999999999994</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B25" s="22">
         <v>2738.4739999999997</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="19" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="24">
+      <c r="A26" s="23">
         <v>56.599999999999994</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="19">
         <v>2738.2259999999997</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="19" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="24">
+      <c r="A27" s="23">
         <v>56.599999999999994</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="19">
         <f>B26-1</f>
         <v>2737.2259999999997</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="19" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>